<commit_message>
Added spreadsheet of Command Tests
</commit_message>
<xml_diff>
--- a/test/Munq.Redis.Tests/Commands/Redis Tests.xlsx
+++ b/test/Munq.Redis.Tests/Commands/Redis Tests.xlsx
@@ -653,7 +653,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,6 +663,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,13 +709,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,19 +1172,19 @@
       <c r="I3" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="7" t="s">
         <v>194</v>
       </c>
     </row>
@@ -1181,19 +1216,19 @@
       <c r="I4" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>195</v>
       </c>
     </row>
@@ -1225,19 +1260,19 @@
       <c r="I5" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="7" t="s">
         <v>196</v>
       </c>
     </row>
@@ -1269,16 +1304,17 @@
       <c r="I6" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="M6" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="7" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1310,16 +1346,17 @@
       <c r="I7" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="M7" t="s">
+      <c r="L7" s="7"/>
+      <c r="M7" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="7" t="s">
         <v>198</v>
       </c>
     </row>
@@ -1339,22 +1376,23 @@
       <c r="F8" t="s">
         <v>102</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H8" t="s">
         <v>136</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="M8" t="s">
+      <c r="L8" s="7"/>
+      <c r="M8" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="7" t="s">
         <v>199</v>
       </c>
     </row>
@@ -1374,13 +1412,13 @@
       <c r="F9" t="s">
         <v>103</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="10" t="s">
         <v>117</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="6" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1394,19 +1432,19 @@
       <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>75</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="6" t="s">
         <v>118</v>
       </c>
       <c r="H10" t="s">
         <v>138</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="6" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1420,19 +1458,19 @@
       <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>76</v>
       </c>
       <c r="F11" t="s">
         <v>105</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="6" t="s">
         <v>119</v>
       </c>
       <c r="H11" t="s">
         <v>139</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="6" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1446,19 +1484,19 @@
       <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>120</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="6" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1472,19 +1510,19 @@
       <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>78</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="10" t="s">
         <v>121</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="6" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1504,13 +1542,13 @@
       <c r="F14" t="s">
         <v>108</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="10" t="s">
         <v>122</v>
       </c>
       <c r="H14" t="s">
         <v>142</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="6" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1530,13 +1568,13 @@
       <c r="F15" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="6" t="s">
         <v>123</v>
       </c>
       <c r="H15" t="s">
         <v>143</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="6" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1556,13 +1594,13 @@
       <c r="F16" t="s">
         <v>110</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="6" t="s">
         <v>126</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="6" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1579,13 +1617,13 @@
       <c r="F17" t="s">
         <v>111</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="6" t="s">
         <v>124</v>
       </c>
       <c r="H17" t="s">
         <v>145</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="6" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1599,13 +1637,13 @@
       <c r="E18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="10" t="s">
         <v>127</v>
       </c>
       <c r="H18" t="s">
         <v>146</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="6" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1616,16 +1654,16 @@
       <c r="D19" t="s">
         <v>67</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="10" t="s">
         <v>128</v>
       </c>
       <c r="H19" t="s">
         <v>147</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="6" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1633,7 +1671,7 @@
       <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="9" t="s">
         <v>85</v>
       </c>
       <c r="G20" t="s">
@@ -1642,7 +1680,7 @@
       <c r="H20" t="s">
         <v>148</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="6" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1653,7 +1691,7 @@
       <c r="E21" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="10" t="s">
         <v>130</v>
       </c>
       <c r="H21" t="s">
@@ -1672,7 +1710,7 @@
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="C23" s="6" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -1702,7 +1740,7 @@
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
+      <c r="E26" s="6" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished update to RC2, all tests passing
</commit_message>
<xml_diff>
--- a/test/Munq.Redis.Tests/Commands/Redis Tests.xlsx
+++ b/test/Munq.Redis.Tests/Commands/Redis Tests.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.OFFICE\Source\Repos\Munq.Redis\test\Munq.Redis.Tests\Commands\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="206">
   <si>
     <t>Cluster</t>
   </si>
@@ -622,12 +627,24 @@
   </si>
   <si>
     <t>FlushDb</t>
+  </si>
+  <si>
+    <t>Hashs</t>
+  </si>
+  <si>
+    <t>HKeys</t>
+  </si>
+  <si>
+    <t>Hlen</t>
+  </si>
+  <si>
+    <t>HSet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -712,8 +729,6 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -721,6 +736,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,14 +766,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:N32" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:N32"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:O32" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:O32"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="Connection"/>
     <tableColumn id="2" name="Hashes"/>
     <tableColumn id="3" name="Keys"/>
@@ -764,6 +784,7 @@
     <tableColumn id="5" name="Server"/>
     <tableColumn id="6" name="Sets"/>
     <tableColumn id="7" name="Sorted Sets"/>
+    <tableColumn id="15" name="Hashs"/>
     <tableColumn id="8" name="Strings"/>
     <tableColumn id="9" name="Transactions"/>
     <tableColumn id="10" name="Cluster"/>
@@ -819,7 +840,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -852,9 +873,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -887,6 +925,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1063,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1133,7 @@
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -1087,77 +1142,80 @@
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F3" t="s">
@@ -1166,80 +1224,86 @@
       <c r="G3" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
         <v>132</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
@@ -1248,39 +1312,42 @@
       <c r="E5" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>99</v>
       </c>
       <c r="G5" t="s">
         <v>113</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
         <v>133</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
@@ -1298,27 +1365,30 @@
       <c r="G6" t="s">
         <v>114</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="L6" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="5"/>
+      <c r="N6" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1334,40 +1404,43 @@
       <c r="E7" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>101</v>
       </c>
       <c r="G7" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="L7" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E8" t="s">
@@ -1376,34 +1449,37 @@
       <c r="F8" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>116</v>
       </c>
       <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
         <v>136</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="L8" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="O8" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E9" t="s">
@@ -1412,18 +1488,21 @@
       <c r="F9" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
@@ -1432,24 +1511,27 @@
       <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I10" t="s">
         <v>138</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="K10" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
@@ -1458,49 +1540,55 @@
       <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>76</v>
       </c>
       <c r="F11" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
         <v>139</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1510,24 +1598,27 @@
       <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
@@ -1542,21 +1633,24 @@
       <c r="F14" t="s">
         <v>108</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="8" t="s">
         <v>122</v>
       </c>
       <c r="H14" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" t="s">
         <v>142</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D15" t="s">
@@ -1565,27 +1659,30 @@
       <c r="E15" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>123</v>
       </c>
       <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
         <v>143</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="K15" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E16" t="s">
@@ -1594,21 +1691,24 @@
       <c r="F16" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="K16" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E17" t="s">
@@ -1617,160 +1717,163 @@
       <c r="F17" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
         <v>145</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="K17" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>146</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="K18" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>45</v>
       </c>
       <c r="D19" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>147</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="K19" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>85</v>
       </c>
       <c r="G20" t="s">
         <v>129</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>148</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="K20" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="6" t="s">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E25" s="5" t="s">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="I25" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E26" s="6" t="s">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E27" s="5" t="s">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E28" s="5" t="s">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E28" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="5" t="s">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="5" t="s">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E32" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1779,8 +1882,9 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>